<commit_message>
Done AND logical operations
</commit_message>
<xml_diff>
--- a/Excel logical practice.xlsx
+++ b/Excel logical practice.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Learning Data analytics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{752A9AB7-C629-4599-8FC6-9FA7EFBA8A00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19A38950-DE8C-4FC2-BE73-3D667EBA5D40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{185D97FB-E57A-40AF-8DED-82FB167AC6E9}"/>
   </bookViews>
@@ -487,8 +487,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:P1471"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L67" sqref="L67"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>